<commit_message>
fix: Balance Fix (보우미터 사거리)
</commit_message>
<xml_diff>
--- a/INFEST_Project/Util/ExcelToJsonWizard.v1.0.6/excel_files/BowmeterSkillTable.xlsx
+++ b/INFEST_Project/Util/ExcelToJsonWizard.v1.0.6/excel_files/BowmeterSkillTable.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\worni\Desktop\GitProject\INFEST\INFEST_Project\Util\ExcelToJsonWizard.v1.0.6\excel_files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{79F2134F-0D24-4DCC-AD26-6A4F75A5FDBD}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{61242092-D2F4-4F22-A822-1481A2AF41E4}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="17025" windowHeight="7875" xr2:uid="{CF8620D6-7292-4E8C-8303-344569A6BA25}"/>
   </bookViews>
@@ -483,7 +483,7 @@
   <dimension ref="A1:F6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E4" sqref="E4"/>
+      <selection activeCell="J5" sqref="J5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -569,7 +569,7 @@
         <v>1</v>
       </c>
       <c r="E4">
-        <v>20</v>
+        <v>10</v>
       </c>
       <c r="F4">
         <v>3</v>
@@ -589,7 +589,7 @@
         <v>7</v>
       </c>
       <c r="E5">
-        <v>25</v>
+        <v>15</v>
       </c>
       <c r="F5">
         <v>2</v>
@@ -609,7 +609,7 @@
         <v>10</v>
       </c>
       <c r="E6">
-        <v>25</v>
+        <v>15</v>
       </c>
       <c r="F6">
         <v>1</v>
@@ -618,5 +618,6 @@
   </sheetData>
   <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>